<commit_message>
add ConnorsRSI indicator (#66)
* add Connor RSI indicator
</commit_message>
<xml_diff>
--- a/IndicatorsTests/Test Data/History.xlsx
+++ b/IndicatorsTests/Test Data/History.xlsx
@@ -2,13 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daves\Repos\Stock.Indicators\IndicatorsTests\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DE2540-07E3-480E-875D-4A8766DB883F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D997E7A-9BB3-47D2-8B8E-CB25214A6784}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -665,71 +666,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -820,6 +756,29 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -963,6 +922,29 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -981,6 +963,25 @@
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -995,44 +996,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8FE8A93B-7DCD-4B08-81FC-F6E776229EB3}" name="testdata" displayName="testdata" ref="A1:I503" totalsRowShown="0" headerRowDxfId="2" dataDxfId="21" headerRowCellStyle="Currency" dataCellStyle="Currency">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8FE8A93B-7DCD-4B08-81FC-F6E776229EB3}" name="testdata" displayName="testdata" ref="A1:I503" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowCellStyle="Currency" dataCellStyle="Currency">
   <sortState ref="B2:I503">
     <sortCondition ref="D2"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{9F699A46-4958-42A4-A5C9-B52EB0EE585B}" name="Index" dataDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="1" xr3:uid="{DD54CCF5-B894-464C-82C5-1C75A48942B7}" name="symbol" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{4C01765B-A5DE-46C8-AA90-F736AC067C2C}" name="code" dataDxfId="20">
+    <tableColumn id="9" xr3:uid="{9F699A46-4958-42A4-A5C9-B52EB0EE585B}" name="Index" dataDxfId="19" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{DD54CCF5-B894-464C-82C5-1C75A48942B7}" name="symbol" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{4C01765B-A5DE-46C8-AA90-F736AC067C2C}" name="code" dataDxfId="17">
       <calculatedColumnFormula>"new Quote { Date = DateTime.Parse("""&amp;TEXT(D2,"yyyy-mm-dd")&amp;"""), Open=(decimal)"&amp;E2&amp;", High=(decimal)"&amp;F2&amp;", Low=(decimal)"&amp;G2&amp;", Close=(decimal)"&amp;H2&amp;", Volume = (long)"&amp;I2&amp;" },"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{870234D4-B88D-4DBC-B1B5-A3A328FCAA43}" name="date" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{EF611352-AF5A-4141-B3FC-D86820A763EA}" name="open" dataDxfId="18" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{74B28648-F2A3-4493-9B04-FE02A7EBAE5E}" name="high" dataDxfId="17" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{F6126363-2529-4BAC-9F69-0710D7A587F6}" name="low" dataDxfId="16" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{1625C5E8-2802-4281-81F5-7308EFB9EB0C}" name="close" dataDxfId="15" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{9D524E41-7E60-45BD-80C8-513C8040D514}" name="volume" dataDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{870234D4-B88D-4DBC-B1B5-A3A328FCAA43}" name="date" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{EF611352-AF5A-4141-B3FC-D86820A763EA}" name="open" dataDxfId="15" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{74B28648-F2A3-4493-9B04-FE02A7EBAE5E}" name="high" dataDxfId="14" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{F6126363-2529-4BAC-9F69-0710D7A587F6}" name="low" dataDxfId="13" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{1625C5E8-2802-4281-81F5-7308EFB9EB0C}" name="close" dataDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{9D524E41-7E60-45BD-80C8-513C8040D514}" name="volume" dataDxfId="11" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C7FBF0C4-2D87-4ACD-AFCE-78C17C20496F}" name="testdata_other" displayName="testdata_other" ref="A1:I503" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="Currency" dataCellStyle="Currency">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C7FBF0C4-2D87-4ACD-AFCE-78C17C20496F}" name="testdata_other" displayName="testdata_other" ref="A1:I503" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowCellStyle="Currency" dataCellStyle="Currency">
   <sortState ref="B2:I503">
     <sortCondition ref="D2"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{09F434F8-2762-4D53-B864-EE5CF712A65F}" name="Index" dataDxfId="0" dataCellStyle="Currency"/>
-    <tableColumn id="1" xr3:uid="{A79861BC-7745-462A-AA04-8C5B139445DD}" name="symbol" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{C0EC46FE-692D-4F84-8E53-54D506FC6C52}" name="code" dataDxfId="11">
+    <tableColumn id="9" xr3:uid="{09F434F8-2762-4D53-B864-EE5CF712A65F}" name="Index" dataDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{A79861BC-7745-462A-AA04-8C5B139445DD}" name="symbol" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{C0EC46FE-692D-4F84-8E53-54D506FC6C52}" name="code" dataDxfId="6">
       <calculatedColumnFormula>"new Quote { Date = DateTime.Parse("""&amp;TEXT(D2,"yyyy-mm-dd")&amp;"""), Open=(decimal)"&amp;E2&amp;", High=(decimal)"&amp;F2&amp;", Low=(decimal)"&amp;G2&amp;", Close=(decimal)"&amp;H2&amp;", Volume = (long)"&amp;I2&amp;" },"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{52C8A72C-9901-43D4-9EFB-6A7DEF9803C8}" name="date" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{ED60DC4C-9D5F-404C-AF5B-D2AB3454BFDC}" name="open" dataDxfId="9" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{6F343C4B-558B-40DD-BDBE-8AC1E73A8A09}" name="high" dataDxfId="8" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{76ACC189-A0C4-41BE-AC4B-E7974CA91250}" name="low" dataDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{064878FE-D3D5-41CB-B806-B4DB1749F21C}" name="close" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{60410A30-408D-4E18-82F8-E1B6AC44D798}" name="volume" dataDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{52C8A72C-9901-43D4-9EFB-6A7DEF9803C8}" name="date" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{ED60DC4C-9D5F-404C-AF5B-D2AB3454BFDC}" name="open" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{6F343C4B-558B-40DD-BDBE-8AC1E73A8A09}" name="high" dataDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{76ACC189-A0C4-41BE-AC4B-E7974CA91250}" name="low" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{064878FE-D3D5-41CB-B806-B4DB1749F21C}" name="close" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{60410A30-408D-4E18-82F8-E1B6AC44D798}" name="volume" dataDxfId="0" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>